<commit_message>
fixed how to measure running time
</commit_message>
<xml_diff>
--- a/cmd/install/performance.xlsx
+++ b/cmd/install/performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dba4cded802036d1/2020년/gRPC 성능 테스트/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gohome\src\github.com\devplayg\grpc-server\cmd\install\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Generator</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -83,6 +83,10 @@
   </si>
   <si>
     <t>Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>worker</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -91,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="182" formatCode="#,##0_ "/>
+    <numFmt numFmtId="176" formatCode="#,##0_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -110,7 +114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,8 +145,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -191,17 +201,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -210,16 +252,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -502,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G20" sqref="G20:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -523,7 +565,7 @@
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -531,297 +573,740 @@
         <v>1042592</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="6" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="G4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5">
+      <c r="L4" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
         <v>10</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <f>A5*B5</f>
         <v>30</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>304</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>2775</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>31277760</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <v>544</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>11</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="3">
         <v>533</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="3">
         <v>31277760</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="3">
         <f>J5/I5*1000</f>
         <v>58682476.547842398</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5">
+      <c r="L5" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
         <v>100</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <f t="shared" ref="C6:C14" si="0">A6*B6</f>
         <v>300</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>12441</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>27692</v>
       </c>
-      <c r="F6" s="5">
-        <v>312777600</v>
-      </c>
-      <c r="G6" s="5">
+      <c r="F6" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="G6" s="3">
         <v>26720</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>137</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>3939</v>
       </c>
-      <c r="J6" s="5">
-        <v>312777600</v>
-      </c>
-      <c r="K6" s="5">
-        <f t="shared" ref="K6:K15" si="1">J6/I6*1000</f>
+      <c r="J6" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" ref="K6:K17" si="1">J6/I6*1000</f>
         <v>79405331.302361012</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <v>3</v>
-      </c>
-      <c r="B7" s="5">
+      <c r="L6" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3">
         <v>100</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>5135</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>28039</v>
       </c>
-      <c r="F7" s="5">
-        <v>312777600</v>
-      </c>
-      <c r="G7" s="5">
+      <c r="F7" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="G7" s="3">
         <v>28565</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>123</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="3">
         <v>4493</v>
       </c>
-      <c r="J7" s="5">
-        <v>312777600</v>
-      </c>
-      <c r="K7" s="5">
+      <c r="J7" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="K7" s="3">
         <f t="shared" si="1"/>
         <v>69614422.434898734</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5">
+      <c r="L7" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
         <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D9" s="3">
+        <v>315</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2857</v>
+      </c>
+      <c r="F9" s="3">
+        <v>31277760</v>
+      </c>
+      <c r="G9" s="3">
+        <v>844</v>
+      </c>
+      <c r="H9" s="3">
+        <v>173</v>
+      </c>
+      <c r="I9" s="3">
+        <v>399</v>
+      </c>
+      <c r="J9" s="3">
+        <v>31277760</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>78390375.939849615</v>
+      </c>
+      <c r="L9" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D10" s="3">
+        <v>307</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3140</v>
+      </c>
+      <c r="F10" s="3">
+        <v>31277760</v>
+      </c>
+      <c r="G10" s="3">
+        <v>777</v>
+      </c>
+      <c r="H10" s="3">
+        <v>420</v>
+      </c>
+      <c r="I10" s="3">
+        <v>461</v>
+      </c>
+      <c r="J10" s="3">
+        <v>31277760</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
+        <v>67847635.574837312</v>
+      </c>
+      <c r="L10" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3">
+        <v>100</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7981</v>
+      </c>
+      <c r="E11" s="3">
+        <v>28084</v>
+      </c>
+      <c r="F11" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="G11" s="3">
+        <v>26226</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2835</v>
+      </c>
+      <c r="I11" s="3">
+        <v>5303</v>
+      </c>
+      <c r="J11" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
+        <v>58981255.892890818</v>
+      </c>
+      <c r="L11" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3">
+        <v>100</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5014</v>
+      </c>
+      <c r="E12" s="3">
+        <v>30127</v>
+      </c>
+      <c r="F12" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="G12" s="3">
+        <v>27172</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3956</v>
+      </c>
+      <c r="I12" s="3">
+        <v>6328</v>
+      </c>
+      <c r="J12" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="1"/>
+        <v>49427560.050568901</v>
+      </c>
+      <c r="L12" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3">
+        <v>100</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2736</v>
+      </c>
+      <c r="E13" s="3">
+        <v>38347</v>
+      </c>
+      <c r="F13" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="G13" s="3">
+        <v>12258</v>
+      </c>
+      <c r="H13" s="3">
+        <v>5192</v>
+      </c>
+      <c r="I13" s="3">
+        <v>5949</v>
+      </c>
+      <c r="J13" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="1"/>
+        <v>52576500.252143219</v>
+      </c>
+      <c r="L13" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3">
+        <v>100</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2713</v>
+      </c>
+      <c r="E14" s="3">
+        <v>38041</v>
+      </c>
+      <c r="F14" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="G14" s="3">
+        <v>12700</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4526</v>
+      </c>
+      <c r="I14" s="3">
+        <v>4943</v>
+      </c>
+      <c r="J14" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>63276876.390855752</v>
+      </c>
+      <c r="L14" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3">
+        <v>100</v>
+      </c>
+      <c r="C15" s="3">
+        <f>A15*B15</f>
+        <v>300</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2752</v>
+      </c>
+      <c r="E15" s="3">
+        <v>34593</v>
+      </c>
+      <c r="F15" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="G15" s="3">
+        <v>13256</v>
+      </c>
+      <c r="H15" s="3">
+        <v>6853</v>
+      </c>
+      <c r="I15" s="3">
+        <v>9477</v>
+      </c>
+      <c r="J15" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="1"/>
+        <v>33003861.981639761</v>
+      </c>
+      <c r="L15" s="11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3">
+        <v>100</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" ref="C16:C26" si="2">A16*B16</f>
+        <v>300</v>
+      </c>
+      <c r="D16" s="3">
+        <v>4522</v>
+      </c>
+      <c r="E16" s="3">
+        <v>28999</v>
+      </c>
+      <c r="F16" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="G16" s="3">
+        <v>23886</v>
+      </c>
+      <c r="H16" s="3">
+        <v>4903</v>
+      </c>
+      <c r="I16" s="3">
+        <v>6494</v>
+      </c>
+      <c r="J16" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="1"/>
+        <v>48164089.929165386</v>
+      </c>
+      <c r="L16" s="11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3">
+        <v>100</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="D17" s="3">
+        <v>4913</v>
+      </c>
+      <c r="E17" s="3">
+        <v>31741</v>
+      </c>
+      <c r="F17" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="G17" s="3">
+        <v>25183</v>
+      </c>
+      <c r="H17" s="3">
+        <v>5141</v>
+      </c>
+      <c r="I17" s="3">
+        <v>7228</v>
+      </c>
+      <c r="J17" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="1"/>
+        <v>43273049.252905369</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>3</v>
+      </c>
+      <c r="B18" s="8">
+        <v>100</v>
+      </c>
+      <c r="C18" s="8">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="D18" s="8">
+        <v>2783</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D19" s="3">
+        <v>306</v>
+      </c>
+      <c r="E19" s="3">
+        <v>281</v>
+      </c>
+      <c r="F19" s="3">
+        <v>31277760</v>
+      </c>
+      <c r="G19" s="3">
+        <v>276</v>
+      </c>
+      <c r="H19" s="3">
+        <v>152</v>
+      </c>
+      <c r="I19" s="3">
+        <v>339</v>
+      </c>
+      <c r="J19" s="3">
+        <v>31277760</v>
+      </c>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3">
+        <v>100</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2774</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2723</v>
+      </c>
+      <c r="F20" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2696</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1748</v>
+      </c>
+      <c r="I20" s="3">
+        <v>3232</v>
+      </c>
+      <c r="J20" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5">
-        <f t="shared" si="0"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5">
-        <f t="shared" si="0"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5">
-        <f t="shared" si="0"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5">
-        <f t="shared" si="0"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5">
-        <f t="shared" si="0"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5">
-        <f>A15*B15</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
added monitoring service to classifier refactored classifier
</commit_message>
<xml_diff>
--- a/cmd/install/performance.xlsx
+++ b/cmd/install/performance.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22875" windowHeight="10005"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22875" windowHeight="10005" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Generator</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -89,15 +90,81 @@
     <t>worker</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Generator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Receiver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Receiver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exec time (ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Upload Sum (ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insert Sum (ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Upload (MBps)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insert (Eps)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
+    <numFmt numFmtId="177" formatCode="#,##0_);[Red]\(#,##0\)"/>
+    <numFmt numFmtId="178" formatCode="#,##0.0_);[Red]\(#,##0.0\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,8 +180,25 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +235,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -221,13 +317,212 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -244,6 +539,156 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -252,16 +697,37 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -544,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:J20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -574,22 +1040,22 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -625,7 +1091,7 @@
       <c r="K4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -665,7 +1131,7 @@
         <f>J5/I5*1000</f>
         <v>58682476.547842398</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="8">
         <v>8</v>
       </c>
     </row>
@@ -702,10 +1168,10 @@
         <v>312777600</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" ref="K6:K17" si="1">J6/I6*1000</f>
+        <f t="shared" ref="K6:K18" si="1">J6/I6*1000</f>
         <v>79405331.302361012</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="8">
         <v>8</v>
       </c>
     </row>
@@ -745,24 +1211,24 @@
         <f t="shared" si="1"/>
         <v>69614422.434898734</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="8">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -801,7 +1267,7 @@
         <f t="shared" si="1"/>
         <v>78390375.939849615</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="9">
         <v>8</v>
       </c>
     </row>
@@ -841,7 +1307,7 @@
         <f t="shared" si="1"/>
         <v>67847635.574837312</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="9">
         <v>8</v>
       </c>
     </row>
@@ -881,7 +1347,7 @@
         <f t="shared" si="1"/>
         <v>58981255.892890818</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="9">
         <v>8</v>
       </c>
     </row>
@@ -921,7 +1387,7 @@
         <f t="shared" si="1"/>
         <v>49427560.050568901</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="9">
         <v>8</v>
       </c>
     </row>
@@ -961,7 +1427,7 @@
         <f t="shared" si="1"/>
         <v>52576500.252143219</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="8">
         <v>16</v>
       </c>
     </row>
@@ -1001,7 +1467,7 @@
         <f t="shared" si="1"/>
         <v>63276876.390855752</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="8">
         <v>16</v>
       </c>
     </row>
@@ -1013,206 +1479,173 @@
         <v>100</v>
       </c>
       <c r="C15" s="3">
-        <f>A15*B15</f>
+        <f t="shared" ref="C15:C24" si="2">A15*B15</f>
         <v>300</v>
       </c>
       <c r="D15" s="3">
-        <v>2752</v>
+        <v>4522</v>
       </c>
       <c r="E15" s="3">
-        <v>34593</v>
+        <v>28999</v>
       </c>
       <c r="F15" s="3">
         <v>312777600</v>
       </c>
       <c r="G15" s="3">
-        <v>13256</v>
+        <v>23886</v>
       </c>
       <c r="H15" s="3">
-        <v>6853</v>
+        <v>4903</v>
       </c>
       <c r="I15" s="3">
-        <v>9477</v>
+        <v>6494</v>
       </c>
       <c r="J15" s="3">
         <v>312777600</v>
       </c>
       <c r="K15" s="3">
         <f t="shared" si="1"/>
-        <v>33003861.981639761</v>
-      </c>
-      <c r="L15" s="11">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+        <v>48164089.929165386</v>
+      </c>
+      <c r="L15" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
         <v>3</v>
       </c>
-      <c r="B16" s="3">
-        <v>100</v>
-      </c>
-      <c r="C16" s="3">
-        <f t="shared" ref="C16:C26" si="2">A16*B16</f>
+      <c r="B16" s="6">
+        <v>100</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
-      <c r="D16" s="3">
-        <v>4522</v>
-      </c>
-      <c r="E16" s="3">
-        <v>28999</v>
-      </c>
-      <c r="F16" s="3">
-        <v>312777600</v>
-      </c>
-      <c r="G16" s="3">
-        <v>23886</v>
-      </c>
-      <c r="H16" s="3">
-        <v>4903</v>
-      </c>
-      <c r="I16" s="3">
-        <v>6494</v>
-      </c>
-      <c r="J16" s="3">
-        <v>312777600</v>
-      </c>
-      <c r="K16" s="3">
-        <f t="shared" si="1"/>
-        <v>48164089.929165386</v>
-      </c>
-      <c r="L16" s="11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D16" s="6">
+        <v>2783</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>3</v>
       </c>
       <c r="B17" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="D17" s="3">
-        <v>4913</v>
+        <v>515</v>
       </c>
       <c r="E17" s="3">
-        <v>31741</v>
+        <v>458</v>
       </c>
       <c r="F17" s="3">
-        <v>312777600</v>
+        <v>31277760</v>
       </c>
       <c r="G17" s="3">
-        <v>25183</v>
+        <v>449</v>
       </c>
       <c r="H17" s="3">
-        <v>5141</v>
+        <v>145</v>
       </c>
       <c r="I17" s="3">
-        <v>7228</v>
+        <v>357</v>
       </c>
       <c r="J17" s="3">
-        <v>312777600</v>
+        <v>31277760</v>
       </c>
       <c r="K17" s="3">
         <f t="shared" si="1"/>
-        <v>43273049.252905369</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
+        <v>87612773.109243706</v>
+      </c>
+      <c r="L17" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>3</v>
       </c>
-      <c r="B18" s="8">
-        <v>100</v>
-      </c>
-      <c r="C18" s="8">
+      <c r="B18" s="3">
+        <v>100</v>
+      </c>
+      <c r="C18" s="3">
         <f t="shared" si="2"/>
         <v>300</v>
       </c>
-      <c r="D18" s="8">
-        <v>2783</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>3</v>
-      </c>
-      <c r="B19" s="3">
-        <v>10</v>
-      </c>
+      <c r="D18" s="3">
+        <v>2788</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2740</v>
+      </c>
+      <c r="F18" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2719</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1438</v>
+      </c>
+      <c r="I18" s="3">
+        <v>2942</v>
+      </c>
+      <c r="J18" s="3">
+        <v>312777600</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="1"/>
+        <v>106314615.90754588</v>
+      </c>
+      <c r="L18" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="3">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="D19" s="3">
-        <v>306</v>
-      </c>
-      <c r="E19" s="3">
-        <v>281</v>
-      </c>
-      <c r="F19" s="3">
-        <v>31277760</v>
-      </c>
-      <c r="G19" s="3">
-        <v>276</v>
-      </c>
-      <c r="H19" s="3">
-        <v>152</v>
-      </c>
-      <c r="I19" s="3">
-        <v>339</v>
-      </c>
-      <c r="J19" s="3">
-        <v>31277760</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>3</v>
-      </c>
-      <c r="B20" s="3">
-        <v>100</v>
-      </c>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="3">
         <f t="shared" si="2"/>
-        <v>300</v>
-      </c>
-      <c r="D20" s="3">
-        <v>2774</v>
-      </c>
-      <c r="E20" s="3">
-        <v>2723</v>
-      </c>
-      <c r="F20" s="3">
-        <v>312777600</v>
-      </c>
-      <c r="G20" s="3">
-        <v>2696</v>
-      </c>
-      <c r="H20" s="3">
-        <v>1748</v>
-      </c>
-      <c r="I20" s="3">
-        <v>3232</v>
-      </c>
-      <c r="J20" s="3">
-        <v>312777600</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
@@ -1228,7 +1661,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3">
@@ -1244,7 +1677,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3">
@@ -1260,7 +1693,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3">
@@ -1275,38 +1708,6 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1317,4 +1718,1423 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Z22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.25" style="10" customWidth="1"/>
+    <col min="16" max="16" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="10">
+        <v>1042592</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="61"/>
+    </row>
+    <row r="4" spans="1:26" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="T4" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28">
+        <v>10</v>
+      </c>
+      <c r="B5" s="28">
+        <v>10</v>
+      </c>
+      <c r="C5" s="18">
+        <v>100</v>
+      </c>
+      <c r="D5" s="18">
+        <v>9035</v>
+      </c>
+      <c r="E5" s="19">
+        <v>104259200</v>
+      </c>
+      <c r="F5" s="20">
+        <v>100</v>
+      </c>
+      <c r="G5" s="18">
+        <v>9560</v>
+      </c>
+      <c r="H5" s="21">
+        <v>104259200</v>
+      </c>
+      <c r="I5" s="22">
+        <v>100</v>
+      </c>
+      <c r="J5" s="18">
+        <v>8401</v>
+      </c>
+      <c r="K5" s="18">
+        <v>104259200</v>
+      </c>
+      <c r="L5" s="18">
+        <v>1499</v>
+      </c>
+      <c r="M5" s="18">
+        <v>634</v>
+      </c>
+      <c r="N5" s="28">
+        <f>K5/L5</f>
+        <v>69552.501667778517</v>
+      </c>
+      <c r="O5" s="29">
+        <f>I5/M5*1000</f>
+        <v>157.72870662460568</v>
+      </c>
+      <c r="P5" s="30">
+        <f>C5/D5*1000</f>
+        <v>11.068068622025455</v>
+      </c>
+      <c r="Q5" s="31">
+        <f t="shared" ref="Q5:Q21" si="0">F5/G5*1000</f>
+        <v>10.460251046025103</v>
+      </c>
+      <c r="R5" s="32">
+        <f t="shared" ref="R5:R21" si="1">I5/J5*1000</f>
+        <v>11.903344839900011</v>
+      </c>
+      <c r="S5" s="33">
+        <v>16</v>
+      </c>
+      <c r="T5" s="28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28">
+        <v>10</v>
+      </c>
+      <c r="B6" s="28">
+        <v>10</v>
+      </c>
+      <c r="C6" s="18">
+        <v>100</v>
+      </c>
+      <c r="D6" s="18">
+        <v>8731</v>
+      </c>
+      <c r="E6" s="19">
+        <v>104259200</v>
+      </c>
+      <c r="F6" s="20">
+        <v>100</v>
+      </c>
+      <c r="G6" s="18">
+        <v>9330</v>
+      </c>
+      <c r="H6" s="21">
+        <v>104259200</v>
+      </c>
+      <c r="I6" s="22">
+        <v>100</v>
+      </c>
+      <c r="J6" s="18">
+        <v>9342</v>
+      </c>
+      <c r="K6" s="18">
+        <v>104259200</v>
+      </c>
+      <c r="L6" s="18">
+        <v>1302</v>
+      </c>
+      <c r="M6" s="18">
+        <v>626</v>
+      </c>
+      <c r="N6" s="28">
+        <f>K6/L6</f>
+        <v>80076.190476190473</v>
+      </c>
+      <c r="O6" s="29">
+        <f>I6/M6*1000</f>
+        <v>159.7444089456869</v>
+      </c>
+      <c r="P6" s="30">
+        <f>C6/D6*1000</f>
+        <v>11.453441759248653</v>
+      </c>
+      <c r="Q6" s="31">
+        <f t="shared" si="0"/>
+        <v>10.718113612004288</v>
+      </c>
+      <c r="R6" s="32">
+        <f t="shared" si="1"/>
+        <v>10.704345964461572</v>
+      </c>
+      <c r="S6" s="33">
+        <v>16</v>
+      </c>
+      <c r="T6" s="28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="28">
+        <v>10</v>
+      </c>
+      <c r="B7" s="28">
+        <v>10</v>
+      </c>
+      <c r="C7" s="18">
+        <v>100</v>
+      </c>
+      <c r="D7" s="18">
+        <v>8484</v>
+      </c>
+      <c r="E7" s="19">
+        <v>104259200</v>
+      </c>
+      <c r="F7" s="20">
+        <v>100</v>
+      </c>
+      <c r="G7" s="18">
+        <v>9304</v>
+      </c>
+      <c r="H7" s="21">
+        <v>104259200</v>
+      </c>
+      <c r="I7" s="22">
+        <v>100</v>
+      </c>
+      <c r="J7" s="18">
+        <v>9313</v>
+      </c>
+      <c r="K7" s="18">
+        <v>104259200</v>
+      </c>
+      <c r="L7" s="18">
+        <v>1429</v>
+      </c>
+      <c r="M7" s="18">
+        <v>750</v>
+      </c>
+      <c r="N7" s="28">
+        <f t="shared" ref="N7:N13" si="2">K7/L7</f>
+        <v>72959.552134359692</v>
+      </c>
+      <c r="O7" s="29">
+        <f t="shared" ref="O7:O13" si="3">I7/M7*1000</f>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="P7" s="30">
+        <f t="shared" ref="P7:P13" si="4">C7/D7*1000</f>
+        <v>11.786892975011787</v>
+      </c>
+      <c r="Q7" s="31">
+        <f t="shared" si="0"/>
+        <v>10.748065348237317</v>
+      </c>
+      <c r="R7" s="32">
+        <f t="shared" si="1"/>
+        <v>10.737678513905294</v>
+      </c>
+      <c r="S7" s="33">
+        <v>16</v>
+      </c>
+      <c r="T7" s="28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="28">
+        <v>10</v>
+      </c>
+      <c r="B8" s="28">
+        <v>10</v>
+      </c>
+      <c r="C8" s="18">
+        <v>100</v>
+      </c>
+      <c r="D8" s="18">
+        <v>7828</v>
+      </c>
+      <c r="E8" s="19">
+        <v>104259200</v>
+      </c>
+      <c r="F8" s="20">
+        <v>100</v>
+      </c>
+      <c r="G8" s="18">
+        <v>9289</v>
+      </c>
+      <c r="H8" s="21">
+        <v>104259200</v>
+      </c>
+      <c r="I8" s="22">
+        <v>100</v>
+      </c>
+      <c r="J8" s="18">
+        <v>9306</v>
+      </c>
+      <c r="K8" s="18">
+        <v>104259200</v>
+      </c>
+      <c r="L8" s="18">
+        <v>1319</v>
+      </c>
+      <c r="M8" s="18">
+        <v>484</v>
+      </c>
+      <c r="N8" s="28">
+        <f t="shared" si="2"/>
+        <v>79044.124336618654</v>
+      </c>
+      <c r="O8" s="29">
+        <f t="shared" si="3"/>
+        <v>206.61157024793388</v>
+      </c>
+      <c r="P8" s="30">
+        <f t="shared" si="4"/>
+        <v>12.774655084312723</v>
+      </c>
+      <c r="Q8" s="31">
+        <f t="shared" si="0"/>
+        <v>10.765421466250404</v>
+      </c>
+      <c r="R8" s="32">
+        <f t="shared" si="1"/>
+        <v>10.745755426606491</v>
+      </c>
+      <c r="S8" s="33">
+        <v>32</v>
+      </c>
+      <c r="T8" s="28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="28">
+        <v>10</v>
+      </c>
+      <c r="B9" s="28">
+        <v>10</v>
+      </c>
+      <c r="C9" s="18">
+        <v>100</v>
+      </c>
+      <c r="D9" s="18">
+        <v>7640</v>
+      </c>
+      <c r="E9" s="19">
+        <v>104259200</v>
+      </c>
+      <c r="F9" s="20">
+        <v>100</v>
+      </c>
+      <c r="G9" s="18">
+        <v>9332</v>
+      </c>
+      <c r="H9" s="21">
+        <v>104259200</v>
+      </c>
+      <c r="I9" s="22">
+        <v>100</v>
+      </c>
+      <c r="J9" s="18">
+        <v>9343</v>
+      </c>
+      <c r="K9" s="18">
+        <v>104259200</v>
+      </c>
+      <c r="L9" s="18">
+        <v>1292</v>
+      </c>
+      <c r="M9" s="18">
+        <v>550</v>
+      </c>
+      <c r="N9" s="28">
+        <f t="shared" si="2"/>
+        <v>80695.975232198136</v>
+      </c>
+      <c r="O9" s="29">
+        <f t="shared" si="3"/>
+        <v>181.81818181818181</v>
+      </c>
+      <c r="P9" s="30">
+        <f t="shared" si="4"/>
+        <v>13.089005235602095</v>
+      </c>
+      <c r="Q9" s="31">
+        <f t="shared" si="0"/>
+        <v>10.715816545220747</v>
+      </c>
+      <c r="R9" s="32">
+        <f t="shared" si="1"/>
+        <v>10.703200256876805</v>
+      </c>
+      <c r="S9" s="33">
+        <v>32</v>
+      </c>
+      <c r="T9" s="28">
+        <v>32</v>
+      </c>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+    </row>
+    <row r="10" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="28">
+        <v>10</v>
+      </c>
+      <c r="B10" s="28">
+        <v>10</v>
+      </c>
+      <c r="C10" s="18">
+        <v>100</v>
+      </c>
+      <c r="D10" s="18">
+        <v>7801</v>
+      </c>
+      <c r="E10" s="19">
+        <v>104259200</v>
+      </c>
+      <c r="F10" s="20">
+        <v>100</v>
+      </c>
+      <c r="G10" s="18">
+        <v>9266</v>
+      </c>
+      <c r="H10" s="21">
+        <v>104259200</v>
+      </c>
+      <c r="I10" s="22">
+        <v>100</v>
+      </c>
+      <c r="J10" s="18">
+        <v>9281</v>
+      </c>
+      <c r="K10" s="18">
+        <v>104259200</v>
+      </c>
+      <c r="L10" s="18">
+        <v>1241</v>
+      </c>
+      <c r="M10" s="18">
+        <v>480</v>
+      </c>
+      <c r="N10" s="28">
+        <f t="shared" si="2"/>
+        <v>84012.248186946017</v>
+      </c>
+      <c r="O10" s="29">
+        <f t="shared" si="3"/>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="P10" s="30">
+        <f t="shared" si="4"/>
+        <v>12.818869375721063</v>
+      </c>
+      <c r="Q10" s="31">
+        <f t="shared" si="0"/>
+        <v>10.792143319663285</v>
+      </c>
+      <c r="R10" s="32">
+        <f t="shared" si="1"/>
+        <v>10.774701002047193</v>
+      </c>
+      <c r="S10" s="33">
+        <v>32</v>
+      </c>
+      <c r="T10" s="28">
+        <v>32</v>
+      </c>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+    </row>
+    <row r="11" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28">
+        <v>10</v>
+      </c>
+      <c r="B11" s="28">
+        <v>10</v>
+      </c>
+      <c r="C11" s="18">
+        <v>100</v>
+      </c>
+      <c r="D11" s="18">
+        <v>6916</v>
+      </c>
+      <c r="E11" s="19">
+        <v>104259200</v>
+      </c>
+      <c r="F11" s="20">
+        <v>100</v>
+      </c>
+      <c r="G11" s="18">
+        <v>9181</v>
+      </c>
+      <c r="H11" s="21">
+        <v>104259200</v>
+      </c>
+      <c r="I11" s="22">
+        <v>100</v>
+      </c>
+      <c r="J11" s="18">
+        <v>5863</v>
+      </c>
+      <c r="K11" s="18">
+        <v>104259200</v>
+      </c>
+      <c r="L11" s="18">
+        <v>1510</v>
+      </c>
+      <c r="M11" s="18">
+        <v>696</v>
+      </c>
+      <c r="N11" s="28">
+        <f t="shared" si="2"/>
+        <v>69045.827814569537</v>
+      </c>
+      <c r="O11" s="29">
+        <f t="shared" si="3"/>
+        <v>143.67816091954023</v>
+      </c>
+      <c r="P11" s="30">
+        <f t="shared" si="4"/>
+        <v>14.459224985540775</v>
+      </c>
+      <c r="Q11" s="31">
+        <f t="shared" si="0"/>
+        <v>10.892059688487093</v>
+      </c>
+      <c r="R11" s="32">
+        <f t="shared" si="1"/>
+        <v>17.056114617090227</v>
+      </c>
+      <c r="S11" s="33">
+        <v>64</v>
+      </c>
+      <c r="T11" s="28">
+        <v>64</v>
+      </c>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+      <c r="Z11"/>
+    </row>
+    <row r="12" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="28">
+        <v>10</v>
+      </c>
+      <c r="B12" s="28">
+        <v>10</v>
+      </c>
+      <c r="C12" s="18">
+        <v>100</v>
+      </c>
+      <c r="D12" s="18">
+        <v>7138</v>
+      </c>
+      <c r="E12" s="19">
+        <v>104259200</v>
+      </c>
+      <c r="F12" s="20">
+        <v>100</v>
+      </c>
+      <c r="G12" s="18">
+        <v>9277</v>
+      </c>
+      <c r="H12" s="21">
+        <v>104259200</v>
+      </c>
+      <c r="I12" s="22">
+        <v>100</v>
+      </c>
+      <c r="J12" s="18">
+        <v>9285</v>
+      </c>
+      <c r="K12" s="18">
+        <v>104259200</v>
+      </c>
+      <c r="L12" s="18">
+        <v>1291</v>
+      </c>
+      <c r="M12" s="18">
+        <v>546</v>
+      </c>
+      <c r="N12" s="28">
+        <f t="shared" si="2"/>
+        <v>80758.481797056549</v>
+      </c>
+      <c r="O12" s="29">
+        <f t="shared" si="3"/>
+        <v>183.15018315018312</v>
+      </c>
+      <c r="P12" s="30">
+        <f t="shared" si="4"/>
+        <v>14.009526478005043</v>
+      </c>
+      <c r="Q12" s="31">
+        <f t="shared" si="0"/>
+        <v>10.779346771585642</v>
+      </c>
+      <c r="R12" s="32">
+        <f t="shared" si="1"/>
+        <v>10.770059235325794</v>
+      </c>
+      <c r="S12" s="33">
+        <v>64</v>
+      </c>
+      <c r="T12" s="28">
+        <v>64</v>
+      </c>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+    </row>
+    <row r="13" spans="1:26" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="39">
+        <v>10</v>
+      </c>
+      <c r="B13" s="39">
+        <v>10</v>
+      </c>
+      <c r="C13" s="34">
+        <v>100</v>
+      </c>
+      <c r="D13" s="34">
+        <v>5927</v>
+      </c>
+      <c r="E13" s="35">
+        <v>104259200</v>
+      </c>
+      <c r="F13" s="36">
+        <v>100</v>
+      </c>
+      <c r="G13" s="34">
+        <v>9261</v>
+      </c>
+      <c r="H13" s="37">
+        <v>104259200</v>
+      </c>
+      <c r="I13" s="38">
+        <v>100</v>
+      </c>
+      <c r="J13" s="34">
+        <v>9267</v>
+      </c>
+      <c r="K13" s="34">
+        <v>104259200</v>
+      </c>
+      <c r="L13" s="34">
+        <v>1247</v>
+      </c>
+      <c r="M13" s="34">
+        <v>541</v>
+      </c>
+      <c r="N13" s="39">
+        <f t="shared" si="2"/>
+        <v>83608.019246190859</v>
+      </c>
+      <c r="O13" s="40">
+        <f t="shared" si="3"/>
+        <v>184.84288354898337</v>
+      </c>
+      <c r="P13" s="41">
+        <f t="shared" si="4"/>
+        <v>16.871941960519656</v>
+      </c>
+      <c r="Q13" s="42">
+        <f t="shared" si="0"/>
+        <v>10.797969981643451</v>
+      </c>
+      <c r="R13" s="43">
+        <f t="shared" si="1"/>
+        <v>10.790978741771879</v>
+      </c>
+      <c r="S13" s="44">
+        <v>64</v>
+      </c>
+      <c r="T13" s="39">
+        <v>64</v>
+      </c>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+    </row>
+    <row r="14" spans="1:26" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45">
+        <v>10</v>
+      </c>
+      <c r="B14" s="45">
+        <v>100</v>
+      </c>
+      <c r="C14" s="51">
+        <v>1000</v>
+      </c>
+      <c r="D14" s="51">
+        <v>92027</v>
+      </c>
+      <c r="E14" s="52">
+        <v>1042592000</v>
+      </c>
+      <c r="F14" s="53">
+        <v>1000</v>
+      </c>
+      <c r="G14" s="51">
+        <v>92760</v>
+      </c>
+      <c r="H14" s="54">
+        <v>1042592000</v>
+      </c>
+      <c r="I14" s="55">
+        <v>1000</v>
+      </c>
+      <c r="J14" s="51">
+        <v>91674</v>
+      </c>
+      <c r="K14" s="51">
+        <v>1042592000</v>
+      </c>
+      <c r="L14" s="51">
+        <v>13258</v>
+      </c>
+      <c r="M14" s="51">
+        <v>5698</v>
+      </c>
+      <c r="N14" s="45">
+        <f>K14/L14</f>
+        <v>78638.708704178614</v>
+      </c>
+      <c r="O14" s="46">
+        <f>I14/M14*1000</f>
+        <v>175.50017550017549</v>
+      </c>
+      <c r="P14" s="47">
+        <f>C14/D14*1000</f>
+        <v>10.86637617221033</v>
+      </c>
+      <c r="Q14" s="48">
+        <f t="shared" si="0"/>
+        <v>10.78050884001725</v>
+      </c>
+      <c r="R14" s="49">
+        <f t="shared" si="1"/>
+        <v>10.90821825163078</v>
+      </c>
+      <c r="S14" s="50">
+        <v>16</v>
+      </c>
+      <c r="T14" s="45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28">
+        <v>10</v>
+      </c>
+      <c r="B15" s="28">
+        <v>100</v>
+      </c>
+      <c r="C15" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D15" s="18">
+        <v>97133</v>
+      </c>
+      <c r="E15" s="19">
+        <v>1042592000</v>
+      </c>
+      <c r="F15" s="20">
+        <v>1000</v>
+      </c>
+      <c r="G15" s="18">
+        <v>98094</v>
+      </c>
+      <c r="H15" s="21">
+        <v>1042592000</v>
+      </c>
+      <c r="I15" s="22">
+        <v>1000</v>
+      </c>
+      <c r="J15" s="18">
+        <v>98122</v>
+      </c>
+      <c r="K15" s="18">
+        <v>1042592000</v>
+      </c>
+      <c r="L15" s="18">
+        <v>13304</v>
+      </c>
+      <c r="M15" s="18">
+        <v>6083</v>
+      </c>
+      <c r="N15" s="28">
+        <f>K15/L15</f>
+        <v>78366.806975345768</v>
+      </c>
+      <c r="O15" s="29">
+        <f>I15/M15*1000</f>
+        <v>164.39256945586058</v>
+      </c>
+      <c r="P15" s="30">
+        <f>C15/D15*1000</f>
+        <v>10.295162303233711</v>
+      </c>
+      <c r="Q15" s="31">
+        <f t="shared" si="0"/>
+        <v>10.19430342324709</v>
+      </c>
+      <c r="R15" s="32">
+        <f t="shared" si="1"/>
+        <v>10.191394386579972</v>
+      </c>
+      <c r="S15" s="33">
+        <v>16</v>
+      </c>
+      <c r="T15" s="28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="28">
+        <v>10</v>
+      </c>
+      <c r="B16" s="28">
+        <v>100</v>
+      </c>
+      <c r="C16" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D16" s="18">
+        <v>94119</v>
+      </c>
+      <c r="E16" s="19">
+        <v>1042592000</v>
+      </c>
+      <c r="F16" s="20">
+        <v>1000</v>
+      </c>
+      <c r="G16" s="18">
+        <v>95057</v>
+      </c>
+      <c r="H16" s="21">
+        <v>1042592000</v>
+      </c>
+      <c r="I16" s="22">
+        <v>1000</v>
+      </c>
+      <c r="J16" s="18">
+        <v>95077</v>
+      </c>
+      <c r="K16" s="18">
+        <v>1042592000</v>
+      </c>
+      <c r="L16" s="18">
+        <v>12850</v>
+      </c>
+      <c r="M16" s="18">
+        <v>5427</v>
+      </c>
+      <c r="N16" s="28">
+        <f t="shared" ref="N16:N21" si="5">K16/L16</f>
+        <v>81135.56420233463</v>
+      </c>
+      <c r="O16" s="29">
+        <f t="shared" ref="O16:O21" si="6">I16/M16*1000</f>
+        <v>184.26386585590566</v>
+      </c>
+      <c r="P16" s="30">
+        <f t="shared" ref="P16:P21" si="7">C16/D16*1000</f>
+        <v>10.624847267820526</v>
+      </c>
+      <c r="Q16" s="31">
+        <f t="shared" si="0"/>
+        <v>10.520003787201363</v>
+      </c>
+      <c r="R16" s="32">
+        <f t="shared" si="1"/>
+        <v>10.517790843211291</v>
+      </c>
+      <c r="S16" s="33">
+        <v>16</v>
+      </c>
+      <c r="T16" s="28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28">
+        <v>10</v>
+      </c>
+      <c r="B17" s="28">
+        <v>100</v>
+      </c>
+      <c r="C17" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D17" s="18">
+        <v>93950</v>
+      </c>
+      <c r="E17" s="19">
+        <v>1042592000</v>
+      </c>
+      <c r="F17" s="20">
+        <v>1000</v>
+      </c>
+      <c r="G17" s="18">
+        <v>95239</v>
+      </c>
+      <c r="H17" s="21">
+        <v>1042592000</v>
+      </c>
+      <c r="I17" s="22">
+        <v>1000</v>
+      </c>
+      <c r="J17" s="18">
+        <v>93143</v>
+      </c>
+      <c r="K17" s="18">
+        <v>1042592000</v>
+      </c>
+      <c r="L17" s="18">
+        <v>14992</v>
+      </c>
+      <c r="M17" s="18">
+        <v>6218</v>
+      </c>
+      <c r="N17" s="28">
+        <f t="shared" si="5"/>
+        <v>69543.223052294561</v>
+      </c>
+      <c r="O17" s="29">
+        <f t="shared" si="6"/>
+        <v>160.82341588935347</v>
+      </c>
+      <c r="P17" s="30">
+        <f t="shared" si="7"/>
+        <v>10.643959552953698</v>
+      </c>
+      <c r="Q17" s="31">
+        <f t="shared" si="0"/>
+        <v>10.499900250947617</v>
+      </c>
+      <c r="R17" s="32">
+        <f t="shared" si="1"/>
+        <v>10.736179852484888</v>
+      </c>
+      <c r="S17" s="33">
+        <v>32</v>
+      </c>
+      <c r="T17" s="28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28">
+        <v>10</v>
+      </c>
+      <c r="B18" s="28">
+        <v>100</v>
+      </c>
+      <c r="C18" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D18" s="18">
+        <v>93376</v>
+      </c>
+      <c r="E18" s="19">
+        <v>1042592000</v>
+      </c>
+      <c r="F18" s="20">
+        <v>1000</v>
+      </c>
+      <c r="G18" s="18">
+        <v>94769</v>
+      </c>
+      <c r="H18" s="21">
+        <v>1042592000</v>
+      </c>
+      <c r="I18" s="22">
+        <v>1000</v>
+      </c>
+      <c r="J18" s="18">
+        <v>93056</v>
+      </c>
+      <c r="K18" s="18">
+        <v>1042592000</v>
+      </c>
+      <c r="L18" s="18">
+        <v>13964</v>
+      </c>
+      <c r="M18" s="18">
+        <v>6010</v>
+      </c>
+      <c r="N18" s="28">
+        <f t="shared" si="5"/>
+        <v>74662.847321684327</v>
+      </c>
+      <c r="O18" s="29">
+        <f t="shared" si="6"/>
+        <v>166.38935108153078</v>
+      </c>
+      <c r="P18" s="30">
+        <f t="shared" si="7"/>
+        <v>10.70938999314599</v>
+      </c>
+      <c r="Q18" s="31">
+        <f t="shared" si="0"/>
+        <v>10.551973746689319</v>
+      </c>
+      <c r="R18" s="32">
+        <f t="shared" si="1"/>
+        <v>10.746217331499313</v>
+      </c>
+      <c r="S18" s="33">
+        <v>32</v>
+      </c>
+      <c r="T18" s="28">
+        <v>32</v>
+      </c>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+    </row>
+    <row r="19" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28">
+        <v>10</v>
+      </c>
+      <c r="B19" s="28">
+        <v>100</v>
+      </c>
+      <c r="C19" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D19" s="18">
+        <v>95508</v>
+      </c>
+      <c r="E19" s="19">
+        <v>1042592000</v>
+      </c>
+      <c r="F19" s="20">
+        <v>1000</v>
+      </c>
+      <c r="G19" s="18">
+        <v>96879</v>
+      </c>
+      <c r="H19" s="21">
+        <v>1042592000</v>
+      </c>
+      <c r="I19" s="22">
+        <v>1000</v>
+      </c>
+      <c r="J19" s="18">
+        <v>96900</v>
+      </c>
+      <c r="K19" s="18">
+        <v>1042592000</v>
+      </c>
+      <c r="L19" s="18">
+        <v>13073</v>
+      </c>
+      <c r="M19" s="18">
+        <v>5691</v>
+      </c>
+      <c r="N19" s="28">
+        <f t="shared" si="5"/>
+        <v>79751.548994109995</v>
+      </c>
+      <c r="O19" s="29">
+        <f t="shared" si="6"/>
+        <v>175.71604287471445</v>
+      </c>
+      <c r="P19" s="30">
+        <f t="shared" si="7"/>
+        <v>10.470327093018387</v>
+      </c>
+      <c r="Q19" s="31">
+        <f t="shared" si="0"/>
+        <v>10.322154440074732</v>
+      </c>
+      <c r="R19" s="32">
+        <f t="shared" si="1"/>
+        <v>10.319917440660475</v>
+      </c>
+      <c r="S19" s="33">
+        <v>32</v>
+      </c>
+      <c r="T19" s="28">
+        <v>32</v>
+      </c>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+    </row>
+    <row r="20" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="28">
+        <v>10</v>
+      </c>
+      <c r="B20" s="28">
+        <v>100</v>
+      </c>
+      <c r="C20" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D20" s="18">
+        <v>91511</v>
+      </c>
+      <c r="E20" s="19">
+        <v>1042592000</v>
+      </c>
+      <c r="F20" s="20">
+        <v>1000</v>
+      </c>
+      <c r="G20" s="18">
+        <v>94651</v>
+      </c>
+      <c r="H20" s="21">
+        <v>1042592000</v>
+      </c>
+      <c r="I20" s="22">
+        <v>1000</v>
+      </c>
+      <c r="J20" s="18">
+        <v>94666</v>
+      </c>
+      <c r="K20" s="18">
+        <v>1042592000</v>
+      </c>
+      <c r="L20" s="18">
+        <v>15625</v>
+      </c>
+      <c r="M20" s="18">
+        <v>6927</v>
+      </c>
+      <c r="N20" s="28">
+        <f t="shared" si="5"/>
+        <v>66725.888000000006</v>
+      </c>
+      <c r="O20" s="29">
+        <f t="shared" si="6"/>
+        <v>144.36263894903999</v>
+      </c>
+      <c r="P20" s="30">
+        <f t="shared" si="7"/>
+        <v>10.927648042311853</v>
+      </c>
+      <c r="Q20" s="31">
+        <f t="shared" si="0"/>
+        <v>10.56512873609365</v>
+      </c>
+      <c r="R20" s="32">
+        <f t="shared" si="1"/>
+        <v>10.563454672216002</v>
+      </c>
+      <c r="S20" s="33">
+        <v>64</v>
+      </c>
+      <c r="T20" s="28">
+        <v>64</v>
+      </c>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+    </row>
+    <row r="21" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28">
+        <v>10</v>
+      </c>
+      <c r="B21" s="28">
+        <v>100</v>
+      </c>
+      <c r="C21" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D21" s="18">
+        <v>88789</v>
+      </c>
+      <c r="E21" s="19">
+        <v>1042592000</v>
+      </c>
+      <c r="F21" s="20">
+        <v>1000</v>
+      </c>
+      <c r="G21" s="18">
+        <v>91974</v>
+      </c>
+      <c r="H21" s="21">
+        <v>1042592000</v>
+      </c>
+      <c r="I21" s="22">
+        <v>1000</v>
+      </c>
+      <c r="J21" s="18">
+        <v>91994</v>
+      </c>
+      <c r="K21" s="18">
+        <v>1042592000</v>
+      </c>
+      <c r="L21" s="18">
+        <v>14644</v>
+      </c>
+      <c r="M21" s="18">
+        <v>5888</v>
+      </c>
+      <c r="N21" s="28">
+        <f t="shared" si="5"/>
+        <v>71195.848128926518</v>
+      </c>
+      <c r="O21" s="29">
+        <f t="shared" si="6"/>
+        <v>169.83695652173913</v>
+      </c>
+      <c r="P21" s="30">
+        <f t="shared" si="7"/>
+        <v>11.262656410140897</v>
+      </c>
+      <c r="Q21" s="31">
+        <f t="shared" si="0"/>
+        <v>10.872637919412007</v>
+      </c>
+      <c r="R21" s="32">
+        <f t="shared" si="1"/>
+        <v>10.870274148314021</v>
+      </c>
+      <c r="S21" s="33">
+        <v>64</v>
+      </c>
+      <c r="T21" s="28">
+        <v>64</v>
+      </c>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+    </row>
+    <row r="22" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="28">
+        <v>10</v>
+      </c>
+      <c r="B22" s="28">
+        <v>100</v>
+      </c>
+      <c r="C22" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D22" s="18">
+        <v>89275</v>
+      </c>
+      <c r="E22" s="19">
+        <v>1042592000</v>
+      </c>
+      <c r="F22" s="20">
+        <v>1000</v>
+      </c>
+      <c r="G22" s="18">
+        <v>92857</v>
+      </c>
+      <c r="H22" s="21">
+        <v>1042592000</v>
+      </c>
+      <c r="I22" s="22">
+        <v>1000</v>
+      </c>
+      <c r="J22" s="18">
+        <v>92961</v>
+      </c>
+      <c r="K22" s="18">
+        <v>1042592000</v>
+      </c>
+      <c r="L22" s="18">
+        <v>13499</v>
+      </c>
+      <c r="M22" s="18">
+        <v>6838</v>
+      </c>
+      <c r="N22" s="28">
+        <f t="shared" ref="N22" si="8">K22/L22</f>
+        <v>77234.758130231872</v>
+      </c>
+      <c r="O22" s="29">
+        <f t="shared" ref="O22" si="9">I22/M22*1000</f>
+        <v>146.24159110851127</v>
+      </c>
+      <c r="P22" s="30">
+        <f t="shared" ref="P22" si="10">C22/D22*1000</f>
+        <v>11.201344161299357</v>
+      </c>
+      <c r="Q22" s="31">
+        <f t="shared" ref="Q22" si="11">F22/G22*1000</f>
+        <v>10.769247337303595</v>
+      </c>
+      <c r="R22" s="32">
+        <f t="shared" ref="R22" si="12">I22/J22*1000</f>
+        <v>10.757199255601812</v>
+      </c>
+      <c r="S22" s="33">
+        <v>64</v>
+      </c>
+      <c r="T22" s="28">
+        <v>64</v>
+      </c>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:O3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>